<commit_message>
group box drawing, db loading
</commit_message>
<xml_diff>
--- a/2022-world-cup.xlsx
+++ b/2022-world-cup.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruceo\Documents\code\world-cup-poster\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruceo\Documents\code\soccer-tourney-poster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804A4AE9-7582-4F21-879E-ABCD0378FF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA29A3A5-7C47-4BEA-9343-D19661ACED8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
+    <workbookView xWindow="4207" yWindow="3780" windowWidth="19200" windowHeight="10020" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Matches" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="235">
   <si>
     <t>A1</t>
   </si>
@@ -308,9 +308,6 @@
     <t>Senegal</t>
   </si>
   <si>
-    <t>IR Iran</t>
-  </si>
-  <si>
     <t>Peru</t>
   </si>
   <si>
@@ -599,9 +596,6 @@
     <t>RUS</t>
   </si>
   <si>
-    <t>CAM</t>
-  </si>
-  <si>
     <t>CAN</t>
   </si>
   <si>
@@ -744,6 +738,12 @@
   </si>
   <si>
     <t>NED</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>CMR</t>
   </si>
 </sst>
 </file>
@@ -751,12 +751,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -784,12 +790,19 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -829,11 +842,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{800F8CDB-7AF5-47FF-9B24-ABA18C14F7CF}" name="groups" displayName="groups" ref="A1:B33" totalsRowShown="0">
-  <autoFilter ref="A1:B33" xr:uid="{800F8CDB-7AF5-47FF-9B24-ABA18C14F7CF}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{800F8CDB-7AF5-47FF-9B24-ABA18C14F7CF}" name="groups" displayName="groups" ref="A1:D33" totalsRowShown="0">
+  <autoFilter ref="A1:D33" xr:uid="{800F8CDB-7AF5-47FF-9B24-ABA18C14F7CF}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C0AEBB99-51D0-46B6-ACD7-C4F2DC461A4C}" name="seed"/>
     <tableColumn id="2" xr3:uid="{4F3769A9-2ECA-4FF2-A664-A0AB0547CF17}" name="rank"/>
+    <tableColumn id="6" xr3:uid="{9939EAC1-70DA-4870-B16B-3148C7C9BC64}" name="abbrev" dataDxfId="0">
+      <calculatedColumnFormula>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{69712765-66F9-4506-BAC0-3C7C3A12DA2C}" name="team" dataDxfId="1">
+      <calculatedColumnFormula>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1149,8 +1168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ABE575-0207-4299-82CD-74F27B6194DA}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50:D65"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2276,8 +2295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74EACD31-13D5-4397-979B-E3BC18FC7A6C}">
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2287,13 +2306,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" t="s">
         <v>148</v>
       </c>
-      <c r="B1" t="s">
-        <v>149</v>
-      </c>
       <c r="C1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.5">
@@ -2304,7 +2323,7 @@
         <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.5">
@@ -2315,7 +2334,7 @@
         <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.5">
@@ -2326,7 +2345,7 @@
         <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.5">
@@ -2337,7 +2356,7 @@
         <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.5">
@@ -2348,7 +2367,7 @@
         <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.5">
@@ -2359,7 +2378,7 @@
         <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.5">
@@ -2370,7 +2389,7 @@
         <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.5">
@@ -2381,7 +2400,7 @@
         <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.5">
@@ -2392,7 +2411,7 @@
         <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.5">
@@ -2403,7 +2422,7 @@
         <v>78</v>
       </c>
       <c r="C11" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.5">
@@ -2414,7 +2433,7 @@
         <v>79</v>
       </c>
       <c r="C12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.5">
@@ -2425,7 +2444,7 @@
         <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.5">
@@ -2436,7 +2455,7 @@
         <v>81</v>
       </c>
       <c r="C14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.5">
@@ -2447,7 +2466,7 @@
         <v>82</v>
       </c>
       <c r="C15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.5">
@@ -2469,7 +2488,7 @@
         <v>84</v>
       </c>
       <c r="C17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.5">
@@ -2480,7 +2499,7 @@
         <v>85</v>
       </c>
       <c r="C18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.5">
@@ -2491,7 +2510,7 @@
         <v>86</v>
       </c>
       <c r="C19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.5">
@@ -2502,7 +2521,7 @@
         <v>87</v>
       </c>
       <c r="C20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.5">
@@ -2513,7 +2532,7 @@
         <v>88</v>
       </c>
       <c r="C21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.5">
@@ -2521,10 +2540,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>233</v>
       </c>
       <c r="C22" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.5">
@@ -2532,10 +2551,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.5">
@@ -2543,10 +2562,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.5">
@@ -2554,10 +2573,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.5">
@@ -2565,10 +2584,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.5">
@@ -2576,10 +2595,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.5">
@@ -2587,10 +2606,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.5">
@@ -2598,10 +2617,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.5">
@@ -2609,10 +2628,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C30" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.5">
@@ -2620,10 +2639,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.5">
@@ -2631,10 +2650,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C32" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.5">
@@ -2642,10 +2661,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.5">
@@ -2653,10 +2672,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.5">
@@ -2664,10 +2683,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C35" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.5">
@@ -2675,10 +2694,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C36" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.5">
@@ -2686,10 +2705,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.5">
@@ -2697,10 +2716,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C38" t="s">
-        <v>186</v>
+        <v>234</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.5">
@@ -2708,10 +2727,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C39" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.5">
@@ -2719,10 +2738,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C40" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.5">
@@ -2730,10 +2749,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C41" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.5">
@@ -2741,10 +2760,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C42" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.5">
@@ -2752,10 +2771,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C43" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.5">
@@ -2763,10 +2782,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C44" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.5">
@@ -2774,10 +2793,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C45" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.5">
@@ -2785,10 +2804,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C46" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.5">
@@ -2796,10 +2815,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C47" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.5">
@@ -2807,10 +2826,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C48" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.5">
@@ -2818,10 +2837,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C49" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.5">
@@ -2829,10 +2848,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C50" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.5">
@@ -2840,10 +2859,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C51" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.5">
@@ -2851,10 +2870,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C52" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.5">
@@ -2862,10 +2881,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C53" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.5">
@@ -2873,10 +2892,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C54" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.5">
@@ -2884,10 +2903,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C55" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.5">
@@ -2895,10 +2914,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C56" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.5">
@@ -2906,10 +2925,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C57" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.5">
@@ -2917,10 +2936,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C58" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.5">
@@ -2928,10 +2947,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C59" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.5">
@@ -2939,10 +2958,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C60" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.5">
@@ -2950,10 +2969,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C61" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.5">
@@ -2961,10 +2980,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C62" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.5">
@@ -2972,10 +2991,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C63" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.5">
@@ -2983,10 +3002,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C64" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.5">
@@ -2994,10 +3013,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C65" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.5">
@@ -3005,10 +3024,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C66" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.5">
@@ -3016,10 +3035,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C67" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.5">
@@ -3027,10 +3046,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C68" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.5">
@@ -3038,10 +3057,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C69" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.5">
@@ -3049,10 +3068,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C70" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.5">
@@ -3060,10 +3079,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C71" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.5">
@@ -3071,10 +3090,10 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C72" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.5">
@@ -3082,10 +3101,10 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C73" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.5">
@@ -3093,10 +3112,10 @@
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C74" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.5">
@@ -3104,10 +3123,10 @@
         <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C75" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.5">
@@ -3115,10 +3134,10 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C76" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.5">
@@ -3126,10 +3145,10 @@
         <v>82</v>
       </c>
       <c r="B77" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C77" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.5">
@@ -3137,10 +3156,10 @@
         <v>89</v>
       </c>
       <c r="B78" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C78" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.5">
@@ -3148,10 +3167,10 @@
         <v>92</v>
       </c>
       <c r="B79" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C79" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.5">
@@ -3159,10 +3178,10 @@
         <v>93</v>
       </c>
       <c r="B80" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C80" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3175,279 +3194,545 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7827E4A0-E10B-4512-807E-A38B484A1AB9}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B33"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="4" max="4" width="10.64453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" t="s">
         <v>159</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C2" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>QAT</v>
+      </c>
+      <c r="D2" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Qatar</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C3" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>ECU</v>
+      </c>
+      <c r="D3" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Ecuador</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C4" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>SEN</v>
+      </c>
+      <c r="D4" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Senegal</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C5" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>NED</v>
+      </c>
+      <c r="D5" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Netherlands</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C6" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>ENG</v>
+      </c>
+      <c r="D6" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>England</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C7" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>IRN</v>
+      </c>
+      <c r="D7" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Iran</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C8" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>USA</v>
+      </c>
+      <c r="D8" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C9" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>WAL</v>
+      </c>
+      <c r="D9" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Wales</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C10" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>ARG</v>
+      </c>
+      <c r="D10" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Argentina</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11">
         <v>49</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C11" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>KSA</v>
+      </c>
+      <c r="D11" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Saudi Arabia</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C12" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>MEX</v>
+      </c>
+      <c r="D12" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Mexico</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C13" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>POL</v>
+      </c>
+      <c r="D13" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Poland</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>8</v>
       </c>
       <c r="B14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C14" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>FRA</v>
+      </c>
+      <c r="D14" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>France</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>9</v>
       </c>
       <c r="B15">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C15" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>AUS</v>
+      </c>
+      <c r="D15" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Australia</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>10</v>
       </c>
       <c r="B16">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C16" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>DEN</v>
+      </c>
+      <c r="D16" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Denmark</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>11</v>
       </c>
       <c r="B17">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C17" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>TUN</v>
+      </c>
+      <c r="D17" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Tunisia</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C18" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>ESP</v>
+      </c>
+      <c r="D18" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Spain</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C19" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>CRC</v>
+      </c>
+      <c r="D19" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Costa Rica</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C20" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>GER</v>
+      </c>
+      <c r="D20" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Germany</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C21" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>JPN</v>
+      </c>
+      <c r="D21" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Japan</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>16</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C22" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>BEL</v>
+      </c>
+      <c r="D22" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Belgium</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>17</v>
       </c>
       <c r="B23">
         <v>38</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C23" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>CAN</v>
+      </c>
+      <c r="D23" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Canada</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C24" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>MAR</v>
+      </c>
+      <c r="D24" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Morocco</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25">
         <v>16</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C25" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>CRO</v>
+      </c>
+      <c r="D25" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Croatia</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
         <v>30</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C26" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>BRA</v>
+      </c>
+      <c r="D26" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Brazil</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
         <v>31</v>
       </c>
       <c r="B27">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C27" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>SRB</v>
+      </c>
+      <c r="D27" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Serbia</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>24</v>
       </c>
       <c r="B28">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C28" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>SUI</v>
+      </c>
+      <c r="D28" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Switzerland</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
         <v>25</v>
       </c>
       <c r="B29">
         <v>37</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C29" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>CMR</v>
+      </c>
+      <c r="D29" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Cameroon</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C30" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>POR</v>
+      </c>
+      <c r="D30" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Portugal</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31">
         <v>60</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C31" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>GHA</v>
+      </c>
+      <c r="D31" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Ghana</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
         <v>26</v>
       </c>
       <c r="B32">
         <v>13</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="C32" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>URU</v>
+      </c>
+      <c r="D32" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>Uruguay</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>27</v>
       </c>
       <c r="B33">
         <v>29</v>
       </c>
+      <c r="C33" t="str">
+        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>KOR</v>
+      </c>
+      <c r="D33" t="str">
+        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <v>South Korea</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -3473,7 +3758,7 @@
         <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.5">
@@ -3481,7 +3766,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.5">
@@ -3489,7 +3774,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.5">
@@ -3497,7 +3782,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.5">
@@ -3505,7 +3790,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.5">
@@ -3513,7 +3798,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.5">
@@ -3521,7 +3806,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.5">
@@ -3529,7 +3814,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.5">
@@ -3537,7 +3822,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
db refactor; load xlsx instead of yaml
</commit_message>
<xml_diff>
--- a/2022-world-cup.xlsx
+++ b/2022-world-cup.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruceo\Documents\code\soccer-tourney-poster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA29A3A5-7C47-4BEA-9343-D19661ACED8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAA5488-E67C-4E46-99BC-01C7BBF29005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4207" yWindow="3780" windowWidth="19200" windowHeight="10020" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Matches" sheetId="1" r:id="rId1"/>
+    <sheet name="Groups" sheetId="5" r:id="rId1"/>
     <sheet name="Teams" sheetId="2" r:id="rId2"/>
-    <sheet name="Groups" sheetId="3" r:id="rId3"/>
-    <sheet name="Venues" sheetId="4" r:id="rId4"/>
+    <sheet name="Matches" sheetId="1" r:id="rId3"/>
+    <sheet name="Seeds" sheetId="3" r:id="rId4"/>
+    <sheet name="Venues" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="253">
   <si>
     <t>A1</t>
   </si>
@@ -744,6 +745,60 @@
   </si>
   <si>
     <t>CMR</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>#94d9f5</t>
+  </si>
+  <si>
+    <t>#fee289</t>
+  </si>
+  <si>
+    <t>#f79d8f</t>
+  </si>
+  <si>
+    <t>#c4e1b5</t>
+  </si>
+  <si>
+    <t>#b0d0ee</t>
+  </si>
+  <si>
+    <t>#c0e4df</t>
+  </si>
+  <si>
+    <t>#fab077</t>
+  </si>
+  <si>
+    <t>#eecbef</t>
   </si>
 </sst>
 </file>
@@ -816,14 +871,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D36B1D81-AA68-4E33-AA36-B206B4FF7406}" name="matches" displayName="matches" ref="A1:E65" totalsRowShown="0">
-  <autoFilter ref="A1:E65" xr:uid="{D36B1D81-AA68-4E33-AA36-B206B4FF7406}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{35D3E9F5-BB3B-4940-9EB6-C927FD84875C}" name="match"/>
-    <tableColumn id="2" xr3:uid="{97337EE3-AAC3-4452-8381-1A56C6B35138}" name="home"/>
-    <tableColumn id="3" xr3:uid="{AEDB8750-5B25-4357-9054-E49FECC94717}" name="away"/>
-    <tableColumn id="4" xr3:uid="{B178F43D-E631-4314-9E59-2CDA6EDA94F1}" name="time"/>
-    <tableColumn id="5" xr3:uid="{A42548B2-C8DF-4D47-B798-8E23FCB67696}" name="venue"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4B86982E-77B7-4963-838F-4D594C24841B}" name="groups" displayName="groups" ref="A1:B9" totalsRowShown="0">
+  <autoFilter ref="A1:B9" xr:uid="{4B86982E-77B7-4963-838F-4D594C24841B}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{D04AE649-F5C6-439C-82C4-C57814A1DE1E}" name="group"/>
+    <tableColumn id="2" xr3:uid="{2BA5CF03-A322-4826-8CCB-B4F6C812D266}" name="color"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -842,23 +894,37 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{800F8CDB-7AF5-47FF-9B24-ABA18C14F7CF}" name="groups" displayName="groups" ref="A1:D33" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D36B1D81-AA68-4E33-AA36-B206B4FF7406}" name="matches" displayName="matches" ref="A1:E65" totalsRowShown="0">
+  <autoFilter ref="A1:E65" xr:uid="{D36B1D81-AA68-4E33-AA36-B206B4FF7406}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{35D3E9F5-BB3B-4940-9EB6-C927FD84875C}" name="match"/>
+    <tableColumn id="2" xr3:uid="{97337EE3-AAC3-4452-8381-1A56C6B35138}" name="home"/>
+    <tableColumn id="3" xr3:uid="{AEDB8750-5B25-4357-9054-E49FECC94717}" name="away"/>
+    <tableColumn id="4" xr3:uid="{B178F43D-E631-4314-9E59-2CDA6EDA94F1}" name="time"/>
+    <tableColumn id="5" xr3:uid="{A42548B2-C8DF-4D47-B798-8E23FCB67696}" name="venue"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{800F8CDB-7AF5-47FF-9B24-ABA18C14F7CF}" name="seeds" displayName="seeds" ref="A1:D33" totalsRowShown="0">
   <autoFilter ref="A1:D33" xr:uid="{800F8CDB-7AF5-47FF-9B24-ABA18C14F7CF}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C0AEBB99-51D0-46B6-ACD7-C4F2DC461A4C}" name="seed"/>
     <tableColumn id="2" xr3:uid="{4F3769A9-2ECA-4FF2-A664-A0AB0547CF17}" name="rank"/>
-    <tableColumn id="6" xr3:uid="{9939EAC1-70DA-4870-B16B-3148C7C9BC64}" name="abbrev" dataDxfId="0">
-      <calculatedColumnFormula>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{9939EAC1-70DA-4870-B16B-3148C7C9BC64}" name="abbrev" dataDxfId="1">
+      <calculatedColumnFormula>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{69712765-66F9-4506-BAC0-3C7C3A12DA2C}" name="team" dataDxfId="1">
-      <calculatedColumnFormula>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{69712765-66F9-4506-BAC0-3C7C3A12DA2C}" name="team" dataDxfId="0">
+      <calculatedColumnFormula>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9DA10E59-00AC-4E77-BC05-F7C0A6D6D772}" name="venues" displayName="venues" ref="A1:B9" totalsRowShown="0">
   <autoFilter ref="A1:B9" xr:uid="{9DA10E59-00AC-4E77-BC05-F7C0A6D6D772}"/>
   <tableColumns count="2">
@@ -1165,10 +1231,1001 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0914DDE-2044-473C-A566-8D4413C2F6D4}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>241</v>
+      </c>
+      <c r="B6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>242</v>
+      </c>
+      <c r="B7" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>243</v>
+      </c>
+      <c r="B8" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>244</v>
+      </c>
+      <c r="B9" t="s">
+        <v>252</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74EACD31-13D5-4397-979B-E3BC18FC7A6C}">
+  <dimension ref="A1:C80"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="2" max="2" width="14.5859375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>233</v>
+      </c>
+      <c r="C22" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>106</v>
+      </c>
+      <c r="C40" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>112</v>
+      </c>
+      <c r="C46" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>113</v>
+      </c>
+      <c r="C47" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>115</v>
+      </c>
+      <c r="C49" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>116</v>
+      </c>
+      <c r="C50" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>117</v>
+      </c>
+      <c r="C51" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>118</v>
+      </c>
+      <c r="C52" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>119</v>
+      </c>
+      <c r="C53" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>120</v>
+      </c>
+      <c r="C54" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>121</v>
+      </c>
+      <c r="C55" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>123</v>
+      </c>
+      <c r="C57" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>124</v>
+      </c>
+      <c r="C58" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>125</v>
+      </c>
+      <c r="C59" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>126</v>
+      </c>
+      <c r="C60" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>127</v>
+      </c>
+      <c r="C61" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>128</v>
+      </c>
+      <c r="C62" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>129</v>
+      </c>
+      <c r="C63" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>130</v>
+      </c>
+      <c r="C64" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>131</v>
+      </c>
+      <c r="C65" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>132</v>
+      </c>
+      <c r="C66" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>133</v>
+      </c>
+      <c r="C67" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>135</v>
+      </c>
+      <c r="C69" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>136</v>
+      </c>
+      <c r="C70" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>137</v>
+      </c>
+      <c r="C71" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A72">
+        <v>72</v>
+      </c>
+      <c r="B72" t="s">
+        <v>138</v>
+      </c>
+      <c r="C72" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A73">
+        <v>73</v>
+      </c>
+      <c r="B73" t="s">
+        <v>139</v>
+      </c>
+      <c r="C73" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A74">
+        <v>76</v>
+      </c>
+      <c r="B74" t="s">
+        <v>140</v>
+      </c>
+      <c r="C74" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A75">
+        <v>77</v>
+      </c>
+      <c r="B75" t="s">
+        <v>141</v>
+      </c>
+      <c r="C75" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A76">
+        <v>78</v>
+      </c>
+      <c r="B76" t="s">
+        <v>142</v>
+      </c>
+      <c r="C76" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A77">
+        <v>82</v>
+      </c>
+      <c r="B77" t="s">
+        <v>143</v>
+      </c>
+      <c r="C77" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A78">
+        <v>89</v>
+      </c>
+      <c r="B78" t="s">
+        <v>144</v>
+      </c>
+      <c r="C78" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A79">
+        <v>92</v>
+      </c>
+      <c r="B79" t="s">
+        <v>145</v>
+      </c>
+      <c r="C79" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A80">
+        <v>93</v>
+      </c>
+      <c r="B80" t="s">
+        <v>146</v>
+      </c>
+      <c r="C80" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ABE575-0207-4299-82CD-74F27B6194DA}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
@@ -2291,913 +3348,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74EACD31-13D5-4397-979B-E3BC18FC7A6C}">
-  <dimension ref="A1:C80"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
-  <cols>
-    <col min="2" max="2" width="14.5859375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>233</v>
-      </c>
-      <c r="C22" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>89</v>
-      </c>
-      <c r="C23" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>90</v>
-      </c>
-      <c r="C24" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>91</v>
-      </c>
-      <c r="C25" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C26" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>93</v>
-      </c>
-      <c r="C27" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>94</v>
-      </c>
-      <c r="C28" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>95</v>
-      </c>
-      <c r="C29" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>96</v>
-      </c>
-      <c r="C30" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>97</v>
-      </c>
-      <c r="C31" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>98</v>
-      </c>
-      <c r="C32" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>99</v>
-      </c>
-      <c r="C33" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>100</v>
-      </c>
-      <c r="C34" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>101</v>
-      </c>
-      <c r="C35" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>102</v>
-      </c>
-      <c r="C36" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>103</v>
-      </c>
-      <c r="C37" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>104</v>
-      </c>
-      <c r="C38" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>105</v>
-      </c>
-      <c r="C39" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
-        <v>106</v>
-      </c>
-      <c r="C40" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>107</v>
-      </c>
-      <c r="C41" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>108</v>
-      </c>
-      <c r="C42" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43" t="s">
-        <v>109</v>
-      </c>
-      <c r="C43" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44" t="s">
-        <v>110</v>
-      </c>
-      <c r="C44" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>111</v>
-      </c>
-      <c r="C45" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="B46" t="s">
-        <v>112</v>
-      </c>
-      <c r="C46" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>113</v>
-      </c>
-      <c r="C47" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="B48" t="s">
-        <v>114</v>
-      </c>
-      <c r="C48" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="B49" t="s">
-        <v>115</v>
-      </c>
-      <c r="C49" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A50">
-        <v>49</v>
-      </c>
-      <c r="B50" t="s">
-        <v>116</v>
-      </c>
-      <c r="C50" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A51">
-        <v>50</v>
-      </c>
-      <c r="B51" t="s">
-        <v>117</v>
-      </c>
-      <c r="C51" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="B52" t="s">
-        <v>118</v>
-      </c>
-      <c r="C52" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A53">
-        <v>52</v>
-      </c>
-      <c r="B53" t="s">
-        <v>119</v>
-      </c>
-      <c r="C53" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A54">
-        <v>53</v>
-      </c>
-      <c r="B54" t="s">
-        <v>120</v>
-      </c>
-      <c r="C54" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A55">
-        <v>54</v>
-      </c>
-      <c r="B55" t="s">
-        <v>121</v>
-      </c>
-      <c r="C55" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="B56" t="s">
-        <v>122</v>
-      </c>
-      <c r="C56" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A57">
-        <v>56</v>
-      </c>
-      <c r="B57" t="s">
-        <v>123</v>
-      </c>
-      <c r="C57" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A58">
-        <v>57</v>
-      </c>
-      <c r="B58" t="s">
-        <v>124</v>
-      </c>
-      <c r="C58" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A59">
-        <v>58</v>
-      </c>
-      <c r="B59" t="s">
-        <v>125</v>
-      </c>
-      <c r="C59" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A60">
-        <v>59</v>
-      </c>
-      <c r="B60" t="s">
-        <v>126</v>
-      </c>
-      <c r="C60" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="B61" t="s">
-        <v>127</v>
-      </c>
-      <c r="C61" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A62">
-        <v>61</v>
-      </c>
-      <c r="B62" t="s">
-        <v>128</v>
-      </c>
-      <c r="C62" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A63">
-        <v>62</v>
-      </c>
-      <c r="B63" t="s">
-        <v>129</v>
-      </c>
-      <c r="C63" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A64">
-        <v>63</v>
-      </c>
-      <c r="B64" t="s">
-        <v>130</v>
-      </c>
-      <c r="C64" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A65">
-        <v>64</v>
-      </c>
-      <c r="B65" t="s">
-        <v>131</v>
-      </c>
-      <c r="C65" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A66">
-        <v>65</v>
-      </c>
-      <c r="B66" t="s">
-        <v>132</v>
-      </c>
-      <c r="C66" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A67">
-        <v>66</v>
-      </c>
-      <c r="B67" t="s">
-        <v>133</v>
-      </c>
-      <c r="C67" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A68">
-        <v>67</v>
-      </c>
-      <c r="B68" t="s">
-        <v>134</v>
-      </c>
-      <c r="C68" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A69">
-        <v>68</v>
-      </c>
-      <c r="B69" t="s">
-        <v>135</v>
-      </c>
-      <c r="C69" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A70">
-        <v>69</v>
-      </c>
-      <c r="B70" t="s">
-        <v>136</v>
-      </c>
-      <c r="C70" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A71">
-        <v>70</v>
-      </c>
-      <c r="B71" t="s">
-        <v>137</v>
-      </c>
-      <c r="C71" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A72">
-        <v>72</v>
-      </c>
-      <c r="B72" t="s">
-        <v>138</v>
-      </c>
-      <c r="C72" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A73">
-        <v>73</v>
-      </c>
-      <c r="B73" t="s">
-        <v>139</v>
-      </c>
-      <c r="C73" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A74">
-        <v>76</v>
-      </c>
-      <c r="B74" t="s">
-        <v>140</v>
-      </c>
-      <c r="C74" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A75">
-        <v>77</v>
-      </c>
-      <c r="B75" t="s">
-        <v>141</v>
-      </c>
-      <c r="C75" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A76">
-        <v>78</v>
-      </c>
-      <c r="B76" t="s">
-        <v>142</v>
-      </c>
-      <c r="C76" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A77">
-        <v>82</v>
-      </c>
-      <c r="B77" t="s">
-        <v>143</v>
-      </c>
-      <c r="C77" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A78">
-        <v>89</v>
-      </c>
-      <c r="B78" t="s">
-        <v>144</v>
-      </c>
-      <c r="C78" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A79">
-        <v>92</v>
-      </c>
-      <c r="B79" t="s">
-        <v>145</v>
-      </c>
-      <c r="C79" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A80">
-        <v>93</v>
-      </c>
-      <c r="B80" t="s">
-        <v>146</v>
-      </c>
-      <c r="C80" t="s">
-        <v>161</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7827E4A0-E10B-4512-807E-A38B484A1AB9}">
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -3227,11 +3383,11 @@
         <v>51</v>
       </c>
       <c r="C2" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>QAT</v>
       </c>
       <c r="D2" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Qatar</v>
       </c>
     </row>
@@ -3243,11 +3399,11 @@
         <v>46</v>
       </c>
       <c r="C3" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>ECU</v>
       </c>
       <c r="D3" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Ecuador</v>
       </c>
     </row>
@@ -3259,11 +3415,11 @@
         <v>20</v>
       </c>
       <c r="C4" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>SEN</v>
       </c>
       <c r="D4" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Senegal</v>
       </c>
     </row>
@@ -3275,11 +3431,11 @@
         <v>10</v>
       </c>
       <c r="C5" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>NED</v>
       </c>
       <c r="D5" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Netherlands</v>
       </c>
     </row>
@@ -3291,11 +3447,11 @@
         <v>5</v>
       </c>
       <c r="C6" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>ENG</v>
       </c>
       <c r="D6" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>England</v>
       </c>
     </row>
@@ -3307,11 +3463,11 @@
         <v>21</v>
       </c>
       <c r="C7" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>IRN</v>
       </c>
       <c r="D7" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Iran</v>
       </c>
     </row>
@@ -3323,11 +3479,11 @@
         <v>15</v>
       </c>
       <c r="C8" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>USA</v>
       </c>
       <c r="D8" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>USA</v>
       </c>
     </row>
@@ -3339,11 +3495,11 @@
         <v>18</v>
       </c>
       <c r="C9" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>WAL</v>
       </c>
       <c r="D9" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Wales</v>
       </c>
     </row>
@@ -3355,11 +3511,11 @@
         <v>4</v>
       </c>
       <c r="C10" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>ARG</v>
       </c>
       <c r="D10" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Argentina</v>
       </c>
     </row>
@@ -3371,11 +3527,11 @@
         <v>49</v>
       </c>
       <c r="C11" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>KSA</v>
       </c>
       <c r="D11" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Saudi Arabia</v>
       </c>
     </row>
@@ -3387,11 +3543,11 @@
         <v>9</v>
       </c>
       <c r="C12" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>MEX</v>
       </c>
       <c r="D12" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Mexico</v>
       </c>
     </row>
@@ -3403,11 +3559,11 @@
         <v>26</v>
       </c>
       <c r="C13" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>POL</v>
       </c>
       <c r="D13" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Poland</v>
       </c>
     </row>
@@ -3419,11 +3575,11 @@
         <v>3</v>
       </c>
       <c r="C14" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>FRA</v>
       </c>
       <c r="D14" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>France</v>
       </c>
     </row>
@@ -3435,11 +3591,11 @@
         <v>42</v>
       </c>
       <c r="C15" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>AUS</v>
       </c>
       <c r="D15" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Australia</v>
       </c>
     </row>
@@ -3451,11 +3607,11 @@
         <v>11</v>
       </c>
       <c r="C16" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>DEN</v>
       </c>
       <c r="D16" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Denmark</v>
       </c>
     </row>
@@ -3467,11 +3623,11 @@
         <v>35</v>
       </c>
       <c r="C17" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>TUN</v>
       </c>
       <c r="D17" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Tunisia</v>
       </c>
     </row>
@@ -3483,11 +3639,11 @@
         <v>7</v>
       </c>
       <c r="C18" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>ESP</v>
       </c>
       <c r="D18" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Spain</v>
       </c>
     </row>
@@ -3499,11 +3655,11 @@
         <v>31</v>
       </c>
       <c r="C19" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>CRC</v>
       </c>
       <c r="D19" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Costa Rica</v>
       </c>
     </row>
@@ -3515,11 +3671,11 @@
         <v>12</v>
       </c>
       <c r="C20" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>GER</v>
       </c>
       <c r="D20" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Germany</v>
       </c>
     </row>
@@ -3531,11 +3687,11 @@
         <v>23</v>
       </c>
       <c r="C21" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>JPN</v>
       </c>
       <c r="D21" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Japan</v>
       </c>
     </row>
@@ -3547,11 +3703,11 @@
         <v>2</v>
       </c>
       <c r="C22" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>BEL</v>
       </c>
       <c r="D22" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Belgium</v>
       </c>
     </row>
@@ -3563,11 +3719,11 @@
         <v>38</v>
       </c>
       <c r="C23" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>CAN</v>
       </c>
       <c r="D23" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Canada</v>
       </c>
     </row>
@@ -3579,11 +3735,11 @@
         <v>24</v>
       </c>
       <c r="C24" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>MAR</v>
       </c>
       <c r="D24" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Morocco</v>
       </c>
     </row>
@@ -3595,11 +3751,11 @@
         <v>16</v>
       </c>
       <c r="C25" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>CRO</v>
       </c>
       <c r="D25" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Croatia</v>
       </c>
     </row>
@@ -3611,11 +3767,11 @@
         <v>1</v>
       </c>
       <c r="C26" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>BRA</v>
       </c>
       <c r="D26" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Brazil</v>
       </c>
     </row>
@@ -3627,11 +3783,11 @@
         <v>25</v>
       </c>
       <c r="C27" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>SRB</v>
       </c>
       <c r="D27" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Serbia</v>
       </c>
     </row>
@@ -3643,11 +3799,11 @@
         <v>14</v>
       </c>
       <c r="C28" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>SUI</v>
       </c>
       <c r="D28" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Switzerland</v>
       </c>
     </row>
@@ -3659,11 +3815,11 @@
         <v>37</v>
       </c>
       <c r="C29" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>CMR</v>
       </c>
       <c r="D29" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Cameroon</v>
       </c>
     </row>
@@ -3675,11 +3831,11 @@
         <v>8</v>
       </c>
       <c r="C30" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>POR</v>
       </c>
       <c r="D30" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Portugal</v>
       </c>
     </row>
@@ -3691,11 +3847,11 @@
         <v>60</v>
       </c>
       <c r="C31" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>GHA</v>
       </c>
       <c r="D31" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Ghana</v>
       </c>
     </row>
@@ -3707,11 +3863,11 @@
         <v>13</v>
       </c>
       <c r="C32" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>URU</v>
       </c>
       <c r="D32" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>Uruguay</v>
       </c>
     </row>
@@ -3723,11 +3879,11 @@
         <v>29</v>
       </c>
       <c r="C33" t="str">
-        <f>INDEX(teams[abbrev],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[abbrev],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>KOR</v>
       </c>
       <c r="D33" t="str">
-        <f>INDEX(teams[team],MATCH(groups[[#This Row],[rank]],teams[rank]))</f>
+        <f>INDEX(teams[team],MATCH(seeds[[#This Row],[rank]],teams[rank]))</f>
         <v>South Korea</v>
       </c>
     </row>
@@ -3740,7 +3896,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8D127A3-9C04-470D-A669-DED7E035C2BF}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -3750,7 +3906,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="9.05859375" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.46875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
correct RU prefix to L; main.py launching
</commit_message>
<xml_diff>
--- a/2022-world-cup.xlsx
+++ b/2022-world-cup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruceo\Documents\code\soccer-tourney-poster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAA5488-E67C-4E46-99BC-01C7BBF29005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6D8BC2-9CAF-4FFF-9B61-F2C155E72401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
+    <workbookView xWindow="5267" yWindow="3780" windowWidth="18140" windowHeight="10020" activeTab="2" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Groups" sheetId="5" r:id="rId1"/>
@@ -222,12 +222,6 @@
     <t>W60</t>
   </si>
   <si>
-    <t>RU61</t>
-  </si>
-  <si>
-    <t>RU62</t>
-  </si>
-  <si>
     <t>W61</t>
   </si>
   <si>
@@ -799,6 +793,12 @@
   </si>
   <si>
     <t>#eecbef</t>
+  </si>
+  <si>
+    <t>L61</t>
+  </si>
+  <si>
+    <t>L62</t>
   </si>
 </sst>
 </file>
@@ -1234,7 +1234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0914DDE-2044-473C-A566-8D4413C2F6D4}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1242,74 +1242,74 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B7" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B9" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -1335,13 +1335,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.5">
@@ -1349,10 +1349,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.5">
@@ -1360,10 +1360,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.5">
@@ -1371,10 +1371,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.5">
@@ -1382,10 +1382,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.5">
@@ -1393,10 +1393,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.5">
@@ -1404,10 +1404,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.5">
@@ -1415,10 +1415,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.5">
@@ -1426,10 +1426,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.5">
@@ -1437,10 +1437,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.5">
@@ -1448,10 +1448,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.5">
@@ -1459,10 +1459,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.5">
@@ -1470,10 +1470,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.5">
@@ -1481,10 +1481,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.5">
@@ -1492,10 +1492,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.5">
@@ -1503,10 +1503,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.5">
@@ -1514,10 +1514,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.5">
@@ -1525,10 +1525,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.5">
@@ -1536,10 +1536,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C19" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.5">
@@ -1547,10 +1547,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C20" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.5">
@@ -1558,10 +1558,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C21" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.5">
@@ -1569,10 +1569,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C22" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.5">
@@ -1580,10 +1580,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.5">
@@ -1591,10 +1591,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C24" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.5">
@@ -1602,10 +1602,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C25" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.5">
@@ -1613,10 +1613,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.5">
@@ -1624,10 +1624,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C27" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.5">
@@ -1635,10 +1635,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C28" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.5">
@@ -1646,10 +1646,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C29" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.5">
@@ -1657,10 +1657,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C30" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.5">
@@ -1668,10 +1668,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C31" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.5">
@@ -1679,10 +1679,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C32" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.5">
@@ -1690,10 +1690,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C33" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.5">
@@ -1701,10 +1701,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.5">
@@ -1712,10 +1712,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C35" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.5">
@@ -1723,10 +1723,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C36" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.5">
@@ -1734,10 +1734,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C37" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.5">
@@ -1745,10 +1745,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C38" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.5">
@@ -1756,10 +1756,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C39" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.5">
@@ -1767,10 +1767,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C40" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.5">
@@ -1778,10 +1778,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C41" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.5">
@@ -1789,10 +1789,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C42" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.5">
@@ -1800,10 +1800,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C43" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.5">
@@ -1811,10 +1811,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C44" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.5">
@@ -1822,10 +1822,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C45" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.5">
@@ -1833,10 +1833,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C46" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.5">
@@ -1844,10 +1844,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C47" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.5">
@@ -1855,10 +1855,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C48" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.5">
@@ -1866,10 +1866,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C49" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.5">
@@ -1877,10 +1877,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C50" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.5">
@@ -1888,10 +1888,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C51" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.5">
@@ -1899,10 +1899,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C52" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.5">
@@ -1910,10 +1910,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C53" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.5">
@@ -1921,10 +1921,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C54" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.5">
@@ -1932,10 +1932,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C55" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.5">
@@ -1943,10 +1943,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C56" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.5">
@@ -1954,10 +1954,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C57" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.5">
@@ -1965,10 +1965,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C58" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.5">
@@ -1976,10 +1976,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C59" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.5">
@@ -1987,10 +1987,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C60" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.5">
@@ -1998,10 +1998,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C61" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.5">
@@ -2009,10 +2009,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C62" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.5">
@@ -2020,10 +2020,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C63" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.5">
@@ -2031,10 +2031,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C64" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.5">
@@ -2042,10 +2042,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C65" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.5">
@@ -2053,10 +2053,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C66" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.5">
@@ -2064,10 +2064,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C67" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.5">
@@ -2075,10 +2075,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C68" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.5">
@@ -2086,10 +2086,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C69" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.5">
@@ -2097,10 +2097,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C70" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.5">
@@ -2108,10 +2108,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C71" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.5">
@@ -2119,10 +2119,10 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C72" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.5">
@@ -2130,10 +2130,10 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C73" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.5">
@@ -2141,10 +2141,10 @@
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C74" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.5">
@@ -2152,10 +2152,10 @@
         <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C75" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.5">
@@ -2163,10 +2163,10 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C76" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.5">
@@ -2174,10 +2174,10 @@
         <v>82</v>
       </c>
       <c r="B77" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C77" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.5">
@@ -2185,10 +2185,10 @@
         <v>89</v>
       </c>
       <c r="B78" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C78" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.5">
@@ -2196,10 +2196,10 @@
         <v>92</v>
       </c>
       <c r="B79" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C79" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.5">
@@ -2207,10 +2207,10 @@
         <v>93</v>
       </c>
       <c r="B80" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C80" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2225,8 +2225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ABE575-0207-4299-82CD-74F27B6194DA}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2236,19 +2236,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
         <v>64</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>65</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>66</v>
-      </c>
-      <c r="D1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.5">
@@ -3310,10 +3310,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>60</v>
+        <v>251</v>
       </c>
       <c r="C64" t="s">
-        <v>61</v>
+        <v>252</v>
       </c>
       <c r="D64" s="1">
         <v>44912.625</v>
@@ -3327,10 +3327,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C65" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D65" s="1">
         <v>44913.625</v>
@@ -3363,16 +3363,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
@@ -3912,10 +3912,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.5">
@@ -3923,7 +3923,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.5">
@@ -3931,7 +3931,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.5">
@@ -3939,7 +3939,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.5">
@@ -3947,7 +3947,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.5">
@@ -3955,7 +3955,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.5">
@@ -3963,7 +3963,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.5">
@@ -3971,7 +3971,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.5">
@@ -3979,7 +3979,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
japanese translation corrections (thanks ryu!)
</commit_message>
<xml_diff>
--- a/2022-world-cup.xlsx
+++ b/2022-world-cup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruceo\Documents\code\soccer-tourney-poster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B87BF1B-5770-425D-B68D-67B1F52F018E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57C77B6-5882-4CD7-A80C-2EE142E2F820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="5" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
+    <workbookView xWindow="1100" yWindow="1100" windowWidth="19200" windowHeight="10073" activeTab="5" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tournament" sheetId="8" r:id="rId1"/>
@@ -2002,9 +2002,6 @@
     <t>2022 برنامه و کارت امتیاز</t>
   </si>
   <si>
-    <t>2022スケジュールとスコアカード</t>
-  </si>
-  <si>
     <t>مرحله گروهی</t>
   </si>
   <si>
@@ -2036,9 +2033,6 @@
   </si>
   <si>
     <t>نهایی</t>
-  </si>
-  <si>
-    <t>最後の</t>
   </si>
   <si>
     <t>گروه</t>
@@ -2675,6 +2669,42 @@
   <si>
     <t>team.blr</t>
   </si>
+  <si>
+    <r>
+      <t>2022</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="MS Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>年</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="MS Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>杯スケジュールとスコアカード</t>
+    </r>
+  </si>
+  <si>
+    <t>決勝</t>
+  </si>
 </sst>
 </file>
 
@@ -2683,7 +2713,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2702,6 +2732,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="MS Gothic"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2724,10 +2760,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3154,10 +3191,10 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -3204,7 +3241,7 @@
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>593</v>
@@ -3233,10 +3270,10 @@
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>611</v>
@@ -3253,8 +3290,8 @@
       <c r="G3" s="2" t="s">
         <v>615</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>653</v>
+      <c r="H3" t="s">
+        <v>872</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>652</v>
@@ -3283,10 +3320,10 @@
         <v>116</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.5">
@@ -3315,7 +3352,7 @@
         <v>146</v>
       </c>
       <c r="I5" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.5">
@@ -3341,10 +3378,10 @@
         <v>147</v>
       </c>
       <c r="H6" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="I6" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.5">
@@ -3370,10 +3407,10 @@
         <v>148</v>
       </c>
       <c r="H7" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="I7" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.5">
@@ -3399,10 +3436,10 @@
         <v>149</v>
       </c>
       <c r="H8" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="I8" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.5">
@@ -3428,10 +3465,10 @@
         <v>150</v>
       </c>
       <c r="H9" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="I9" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.5">
@@ -3457,10 +3494,10 @@
         <v>592</v>
       </c>
       <c r="H10" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="I10" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.5">
@@ -3486,10 +3523,10 @@
         <v>152</v>
       </c>
       <c r="H11" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="I11" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.5">
@@ -3515,10 +3552,10 @@
         <v>153</v>
       </c>
       <c r="H12" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="I12" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
   </sheetData>
@@ -4314,16 +4351,16 @@
         <v>66</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>849</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>851</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>852</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>854</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>853</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.5">
@@ -6098,10 +6135,10 @@
   <dimension ref="A1:I94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C76" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A93" sqref="A93"/>
+      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -6148,36 +6185,36 @@
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>857</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>859</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>860</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>861</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>862</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>863</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>864</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>865</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>866</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>599</v>
@@ -6198,15 +6235,15 @@
         <v>620</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>600</v>
@@ -6227,15 +6264,15 @@
         <v>625</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>601</v>
@@ -6256,15 +6293,15 @@
         <v>630</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>602</v>
@@ -6285,15 +6322,15 @@
         <v>635</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>603</v>
@@ -6314,15 +6351,15 @@
         <v>640</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>604</v>
@@ -6342,16 +6379,16 @@
       <c r="G8" s="2" t="s">
         <v>642</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>665</v>
+      <c r="H8" s="3" t="s">
+        <v>873</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A9" s="2" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>605</v>
@@ -6372,15 +6409,15 @@
         <v>647</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A10" s="2" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>606</v>
@@ -6403,7 +6440,7 @@
     </row>
     <row r="11" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>607</v>
@@ -6411,7 +6448,7 @@
     </row>
     <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A12" s="2" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>608</v>
@@ -6419,26 +6456,26 @@
     </row>
     <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A13" s="2" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A14" s="2" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A15" s="2" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.5">
@@ -6464,10 +6501,10 @@
         <v>258</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.5">
@@ -6493,10 +6530,10 @@
         <v>263</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.5">
@@ -6522,10 +6559,10 @@
         <v>266</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.5">
@@ -6551,10 +6588,10 @@
         <v>269</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.5">
@@ -6580,10 +6617,10 @@
         <v>273</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.5">
@@ -6609,10 +6646,10 @@
         <v>277</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.5">
@@ -6638,10 +6675,10 @@
         <v>282</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.5">
@@ -6667,10 +6704,10 @@
         <v>74</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.5">
@@ -6696,10 +6733,10 @@
         <v>75</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.5">
@@ -6725,10 +6762,10 @@
         <v>292</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.5">
@@ -6754,10 +6791,10 @@
         <v>297</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.5">
@@ -6783,10 +6820,10 @@
         <v>302</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.5">
@@ -6812,10 +6849,10 @@
         <v>79</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.5">
@@ -6841,10 +6878,10 @@
         <v>307</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.5">
@@ -6870,10 +6907,10 @@
         <v>81</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.5">
@@ -6899,10 +6936,10 @@
         <v>313</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.5">
@@ -6928,10 +6965,10 @@
         <v>83</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.5">
@@ -6957,10 +6994,10 @@
         <v>84</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.5">
@@ -6986,10 +7023,10 @@
         <v>323</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.5">
@@ -7015,10 +7052,10 @@
         <v>86</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.5">
@@ -7044,10 +7081,10 @@
         <v>230</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.5">
@@ -7073,10 +7110,10 @@
         <v>87</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.5">
@@ -7102,10 +7139,10 @@
         <v>88</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.5">
@@ -7131,10 +7168,10 @@
         <v>335</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.5">
@@ -7160,10 +7197,10 @@
         <v>338</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.5">
@@ -7189,10 +7226,10 @@
         <v>341</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.5">
@@ -7218,10 +7255,10 @@
         <v>344</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.5">
@@ -7247,10 +7284,10 @@
         <v>346</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.5">
@@ -7276,10 +7313,10 @@
         <v>351</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.5">
@@ -7305,10 +7342,10 @@
         <v>95</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.5">
@@ -7334,10 +7371,10 @@
         <v>96</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.5">
@@ -7363,10 +7400,10 @@
         <v>354</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.5">
@@ -7392,10 +7429,10 @@
         <v>360</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.5">
@@ -7421,10 +7458,10 @@
         <v>363</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.5">
@@ -7450,10 +7487,10 @@
         <v>367</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.5">
@@ -7479,10 +7516,10 @@
         <v>371</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.5">
@@ -7508,10 +7545,10 @@
         <v>376</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.5">
@@ -7537,10 +7574,10 @@
         <v>103</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.5">
@@ -7566,10 +7603,10 @@
         <v>383</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.5">
@@ -7595,10 +7632,10 @@
         <v>388</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.5">
@@ -7624,10 +7661,10 @@
         <v>393</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.5">
@@ -7653,10 +7690,10 @@
         <v>396</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.5">
@@ -7682,10 +7719,10 @@
         <v>401</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.5">
@@ -7711,10 +7748,10 @@
         <v>405</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.5">
@@ -7740,10 +7777,10 @@
         <v>410</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.5">
@@ -7769,10 +7806,10 @@
         <v>111</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.5">
@@ -7798,10 +7835,10 @@
         <v>415</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.5">
@@ -7827,10 +7864,10 @@
         <v>419</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.5">
@@ -7856,10 +7893,10 @@
         <v>423</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.5">
@@ -7885,10 +7922,10 @@
         <v>115</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.5">
@@ -7914,10 +7951,10 @@
         <v>116</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.5">
@@ -7943,10 +7980,10 @@
         <v>117</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.5">
@@ -7972,10 +8009,10 @@
         <v>429</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.5">
@@ -8001,10 +8038,10 @@
         <v>434</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.5">
@@ -8030,10 +8067,10 @@
         <v>438</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.5">
@@ -8059,10 +8096,10 @@
         <v>121</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.5">
@@ -8088,10 +8125,10 @@
         <v>122</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.5">
@@ -8117,10 +8154,10 @@
         <v>123</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.5">
@@ -8146,10 +8183,10 @@
         <v>446</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.5">
@@ -8175,10 +8212,10 @@
         <v>125</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.5">
@@ -8204,10 +8241,10 @@
         <v>126</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.5">
@@ -8233,10 +8270,10 @@
         <v>452</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.5">
@@ -8262,10 +8299,10 @@
         <v>457</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.5">
@@ -8291,10 +8328,10 @@
         <v>129</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.5">
@@ -8320,10 +8357,10 @@
         <v>464</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.5">
@@ -8349,10 +8386,10 @@
         <v>467</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.5">
@@ -8378,10 +8415,10 @@
         <v>132</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.5">
@@ -8407,10 +8444,10 @@
         <v>473</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.5">
@@ -8436,10 +8473,10 @@
         <v>478</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.5">
@@ -8465,10 +8502,10 @@
         <v>135</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.5">
@@ -8494,10 +8531,10 @@
         <v>480</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.5">
@@ -8523,10 +8560,10 @@
         <v>483</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.5">
@@ -8552,10 +8589,10 @@
         <v>485</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.5">
@@ -8581,10 +8618,10 @@
         <v>139</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.5">
@@ -8610,10 +8647,10 @@
         <v>490</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.5">
@@ -8639,10 +8676,10 @@
         <v>141</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.5">
@@ -8668,10 +8705,10 @@
         <v>491</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.5">
@@ -8697,15 +8734,15 @@
         <v>495</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
     </row>
     <row r="94" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A94" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="B94" t="s">
         <v>144</v>
@@ -8726,10 +8763,10 @@
         <v>500</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
     </row>
   </sheetData>

</xml_diff>